<commit_message>
fix: adjust character mapping
</commit_message>
<xml_diff>
--- a/ocr_dataset.xlsx
+++ b/ocr_dataset.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry James Carlos\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry James Carlos\Desktop\Codes\IAI\ocr-ann\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CE8BA29F-088F-4960-A584-715679C87346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CD6914-B6F6-4E10-B81A-CE07CBAF06E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2130" yWindow="270" windowWidth="23595" windowHeight="14895" xr2:uid="{EC9E1B8A-AEF7-4B97-9F19-7F94773F5E22}"/>
+    <workbookView xWindow="1560" yWindow="1305" windowWidth="23595" windowHeight="14895" xr2:uid="{EC9E1B8A-AEF7-4B97-9F19-7F94773F5E22}"/>
   </bookViews>
   <sheets>
     <sheet name="ocr_dataset" sheetId="1" r:id="rId1"/>
@@ -888,8 +888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95751F20-D723-4984-B789-89D322203DFA}">
   <dimension ref="A1:E288"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A200" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H213" sqref="H213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4149,7 +4149,7 @@
         <v>0</v>
       </c>
       <c r="D210" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E210" s="1">
         <v>1</v>
@@ -4166,7 +4166,7 @@
         <v>0</v>
       </c>
       <c r="D211" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E211" s="1">
         <v>1</v>
@@ -4180,7 +4180,7 @@
         <v>0</v>
       </c>
       <c r="C212" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D212" s="1">
         <v>0</v>
@@ -4194,7 +4194,7 @@
         <v>1</v>
       </c>
       <c r="B213" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C213" s="1">
         <v>0</v>
@@ -4211,7 +4211,7 @@
         <v>1</v>
       </c>
       <c r="B214" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C214" s="1">
         <v>0</v>

</xml_diff>